<commit_message>
despliegue de servicios capa base
</commit_message>
<xml_diff>
--- a/desarrollo-microservicios.xlsx
+++ b/desarrollo-microservicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluismen\Documents\BOOTCAMP-BANK-PROJECT\architecture-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA70614B-5DBB-46C6-88BE-9C5339EC5663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39AF6EF-3B84-4984-ABB7-D08BCCB62010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
+    <workbookView xWindow="3015" yWindow="1920" windowWidth="15375" windowHeight="8850" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <definedName name="col_asignado">Hoja1!$C:$C</definedName>
     <definedName name="col_estado">Hoja1!$E:$E</definedName>
     <definedName name="col_miroservicios">Hoja1!$D:$D</definedName>
-    <definedName name="ln_completed">Hoja1!$K$10</definedName>
-    <definedName name="ln_in_progress">Hoja1!$K$9</definedName>
-    <definedName name="ln_pending">Hoja1!$K$8</definedName>
+    <definedName name="ln_completed">Hoja1!$L$10</definedName>
+    <definedName name="ln_in_progress">Hoja1!$L$9</definedName>
+    <definedName name="ln_pending">Hoja1!$L$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
   <si>
     <t>ms-enterprise-active-credit-card</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>http://config-service.eastus.azurecontainer.io/</t>
+  </si>
+  <si>
+    <t>Github Actions</t>
+  </si>
+  <si>
+    <t>http://gateway-service.eastus.azurecontainer.io/</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -267,326 +283,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1100,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EC3994-2505-4875-A4DA-47990DB02DB0}">
-  <dimension ref="B1:N18"/>
+  <dimension ref="B1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1113,26 +809,26 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="42.140625" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="11.28515625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="44.28515625" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="20.42578125" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="6" max="7" width="11.28515625" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="44.28515625" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="20.42578125" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="N1" s="1">
+    <row r="1" spans="2:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="N2" s="1">
+    <row r="2" spans="2:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1149,14 +845,17 @@
         <v>23</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="2:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -1173,14 +872,17 @@
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>8081</v>
       </c>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="2:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -1197,14 +899,17 @@
         <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>8089</v>
       </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -1218,18 +923,27 @@
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
         <v>16</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -1245,18 +959,21 @@
       <c r="F8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K8" t="s">
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
         <v>15</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="1">
-        <f>COUNTIFS(col_estado,ln_completed,col_asignado,M8)/COUNTIFS(col_asignado,M8)</f>
+      <c r="O8" s="1">
+        <f>COUNTIFS(col_estado,ln_completed,col_asignado,N8)/COUNTIFS(col_asignado,N8)</f>
         <v>0.375</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1272,18 +989,21 @@
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s">
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
         <v>17</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="1">
-        <f>COUNTIFS(col_estado,ln_completed,col_asignado,M9)/COUNTIFS(col_asignado,M9)</f>
+      <c r="O9" s="1">
+        <f>COUNTIFS(col_estado,ln_completed,col_asignado,N9)/COUNTIFS(col_asignado,N9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1299,11 +1019,14 @@
       <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s">
+      <c r="G10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1319,8 +1042,11 @@
       <c r="F11" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -1336,8 +1062,11 @@
       <c r="F13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -1353,8 +1082,11 @@
       <c r="F14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -1370,8 +1102,11 @@
       <c r="F15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -1387,8 +1122,11 @@
       <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -1404,8 +1142,11 @@
       <c r="F17" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -1421,21 +1162,24 @@
       <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K7:K10 E25:H1048576 E7:H20">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+  <conditionalFormatting sqref="L7:L10 E25:I1048576 E7:I20">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N5 N8:N9">
-    <cfRule type="dataBar" priority="18">
+  <conditionalFormatting sqref="O1:O5 O8:O9">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1448,7 +1192,29 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:H3">
+  <conditionalFormatting sqref="E3:I3">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+      <formula>"COMPLETADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+      <formula>"EN PROGRESO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+      <formula>"PENDIENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+      <formula>"COMPLETADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+      <formula>"EN PROGRESO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>"PENDIENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:I5">
     <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
@@ -1459,7 +1225,7 @@
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="E6">
     <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
@@ -1470,7 +1236,7 @@
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:H5">
+  <conditionalFormatting sqref="F6:I6">
     <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
@@ -1481,34 +1247,34 @@
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+  <conditionalFormatting sqref="F1:I1048576">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"SI"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:G6">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:H6">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"PENDIENTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:H1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"SI"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1527,7 +1293,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N1:N5 N8:N9</xm:sqref>
+          <xm:sqref>O1:O5 O8:O9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
ms-enterprise-active-loan deployed on azure with github actions
</commit_message>
<xml_diff>
--- a/desarrollo-microservicios.xlsx
+++ b/desarrollo-microservicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluismen\Documents\BOOTCAMP-BANK-PROJECT\architecture-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39AF6EF-3B84-4984-ABB7-D08BCCB62010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E32C426-02ED-4CC3-98FD-D9FB2AAFE3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="1920" windowWidth="15375" windowHeight="8850" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <definedName name="col_asignado">Hoja1!$C:$C</definedName>
     <definedName name="col_estado">Hoja1!$E:$E</definedName>
     <definedName name="col_miroservicios">Hoja1!$D:$D</definedName>
-    <definedName name="ln_completed">Hoja1!$L$10</definedName>
-    <definedName name="ln_in_progress">Hoja1!$L$9</definedName>
-    <definedName name="ln_pending">Hoja1!$L$8</definedName>
+    <definedName name="ln_completed">Hoja1!$T$10</definedName>
+    <definedName name="ln_in_progress">Hoja1!$T$9</definedName>
+    <definedName name="ln_pending">Hoja1!$T$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="50">
   <si>
     <t>ms-enterprise-active-credit-card</t>
   </si>
@@ -148,13 +148,58 @@
   </si>
   <si>
     <t>http://gateway-service.eastus.azurecontainer.io/</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>Pom</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Config Data</t>
+  </si>
+  <si>
+    <t>Dockerfile</t>
+  </si>
+  <si>
+    <t>README</t>
+  </si>
+  <si>
+    <t>Git Pull</t>
+  </si>
+  <si>
+    <t>CALL TO ACTION</t>
+  </si>
+  <si>
+    <t>http://config-service.eastus.azurecontainer.io:8081</t>
+  </si>
+  <si>
+    <t>http://eureka-service.eastus.azurecontainer.io:8089</t>
+  </si>
+  <si>
+    <t>https://ms-entact-creditcard.azurewebsites.net/enterprise/active/credit_card/docs/ui</t>
+  </si>
+  <si>
+    <t>80:3000</t>
+  </si>
+  <si>
+    <t>https://ms-entact-creditcard.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>https://ms-entact-loan.azurewebsites.net/enterprise/active/loan/docs/ui</t>
+  </si>
+  <si>
+    <t>https://ms-entact-loan.azurewebsites.net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +218,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,11 +254,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -220,12 +274,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -253,126 +311,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -796,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EC3994-2505-4875-A4DA-47990DB02DB0}">
-  <dimension ref="B1:O18"/>
+  <dimension ref="B1:W18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -809,26 +747,34 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="42.140625" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="11.28515625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="44.28515625" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="20.42578125" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="3.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="2.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="11.140625" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="5" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="10.140625" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="8.5703125" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="7.5703125" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="14" width="11.28515625" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="44.85546875" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="20.42578125" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="79.5703125" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="3.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="2.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="O1" s="1">
+    <row r="1" spans="2:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="W1" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="O2" s="1">
+    <row r="2" spans="2:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -842,20 +788,44 @@
         <v>14</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="N3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="2:15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -872,17 +842,41 @@
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="2">
+      <c r="P4" s="2">
         <v>8081</v>
       </c>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="2:15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="2:23" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -899,17 +893,41 @@
         <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="2">
+      <c r="P5" s="2">
         <v>8089</v>
       </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -926,24 +944,48 @@
         <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="2">
+      <c r="P6" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L7" t="s">
+      <c r="Q6" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
         <v>16</v>
       </c>
-      <c r="N7" t="s">
+      <c r="V7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -957,23 +999,53 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" t="s">
         <v>15</v>
       </c>
-      <c r="N8" t="s">
+      <c r="V8" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="1">
-        <f>COUNTIFS(col_estado,ln_completed,col_asignado,N8)/COUNTIFS(col_asignado,N8)</f>
+      <c r="W8" s="1">
+        <f>COUNTIFS(col_estado,ln_completed,col_asignado,V8)/COUNTIFS(col_asignado,V8)</f>
         <v>0.375</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -987,23 +1059,53 @@
         <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" t="s">
         <v>17</v>
       </c>
-      <c r="N9" t="s">
+      <c r="V9" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="1">
-        <f>COUNTIFS(col_estado,ln_completed,col_asignado,N9)/COUNTIFS(col_asignado,N9)</f>
+      <c r="W9" s="1">
+        <f>COUNTIFS(col_estado,ln_completed,col_asignado,V9)/COUNTIFS(col_asignado,V9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1022,11 +1124,32 @@
       <c r="G10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L10" t="s">
+      <c r="H10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1045,8 +1168,29 @@
       <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -1065,8 +1209,29 @@
       <c r="G13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -1085,8 +1250,29 @@
       <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -1105,8 +1291,29 @@
       <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -1125,8 +1332,29 @@
       <c r="G16" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -1145,8 +1373,29 @@
       <c r="G17" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -1165,20 +1414,41 @@
       <c r="G18" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L7:L10 E25:I1048576 E7:I20">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+  <conditionalFormatting sqref="T7:T10 E7:E20 E5 E25:Q1048576 E3:Q3 F5:Q20">
+    <cfRule type="cellIs" dxfId="13" priority="25" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="26" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="27" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O5 O8:O9">
+  <conditionalFormatting sqref="W1:W5 W8:W9">
     <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
@@ -1192,81 +1462,37 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:I3">
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
-      <formula>"PENDIENTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
-      <formula>"COMPLETADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
-      <formula>"EN PROGRESO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
-      <formula>"PENDIENTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:I5">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
-      <formula>"COMPLETADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
-      <formula>"EN PROGRESO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:I6">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
-      <formula>"COMPLETADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>"EN PROGRESO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
-      <formula>"PENDIENTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:I1048576">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="F1:Q1048576">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:G6">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>"COMPLETADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"EN PROGRESO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"PENDIENTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
+  <conditionalFormatting sqref="O6">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
@@ -1277,8 +1503,15 @@
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="Q4" r:id="rId1" xr:uid="{B1687B75-BE1B-4A99-A813-2CE3CADBFBC1}"/>
+    <hyperlink ref="Q5" r:id="rId2" xr:uid="{E76B30F2-5674-4B8C-AA74-CE9CA2A02814}"/>
+    <hyperlink ref="Q6" r:id="rId3" xr:uid="{663091C1-4911-43E1-B1A7-EBAF0C2E35B9}"/>
+    <hyperlink ref="Q8" r:id="rId4" xr:uid="{0A5FA214-80C8-42BF-AF55-52E5F465E622}"/>
+    <hyperlink ref="Q9" r:id="rId5" xr:uid="{EF706626-C987-45E7-8F95-F7F6A1D74B16}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1293,7 +1526,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>O1:O5 O8:O9</xm:sqref>
+          <xm:sqref>W1:W5 W8:W9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
all microservices deployed, 3 standby
</commit_message>
<xml_diff>
--- a/desarrollo-microservicios.xlsx
+++ b/desarrollo-microservicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluismen\Documents\BOOTCAMP-BANK-PROJECT\architecture-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BAE097-B297-4116-96B8-BFB6ECE48A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE75EF3-F0B4-4645-8B2C-EB89D419D39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="96">
   <si>
     <t>ms-enterprise-active-credit-card</t>
   </si>
@@ -295,6 +295,42 @@
   </si>
   <si>
     <t>http://gateway-service.eastus.azurecontainer.io/personal/passive/current_account/docs/ui</t>
+  </si>
+  <si>
+    <t>ms-perpas-fta</t>
+  </si>
+  <si>
+    <t>ms-perpas-savingaccount</t>
+  </si>
+  <si>
+    <t>https://ms-perpas-fta.azurewebsites.net/</t>
+  </si>
+  <si>
+    <t>https://ms-perpas-fta.azurewebsites.net/personal/passive/fixed_term_account/docs/ui</t>
+  </si>
+  <si>
+    <t>http://gateway-service.eastus.azurecontainer.io/personal/passive/fixed_term_account/docs/ui</t>
+  </si>
+  <si>
+    <t>https://ms-perpas-savingaccount.azurewebsites.net/</t>
+  </si>
+  <si>
+    <t>https://ms-perpas-savingaccount.azurewebsites.net/personal/passive/saving_account/docs/ui</t>
+  </si>
+  <si>
+    <t>http://gateway-service.eastus.azurecontainer.io/personal/passive/saving_account/docs/ui</t>
+  </si>
+  <si>
+    <t>ms-perpas-vipsa</t>
+  </si>
+  <si>
+    <t>https://ms-perpas-vipsa.azurewebsites.net/</t>
+  </si>
+  <si>
+    <t>https://ms-perpas-vipsa.azurewebsites.net/personal/passive/vip_saving_account/docs/ui</t>
+  </si>
+  <si>
+    <t>http://gateway-service.eastus.azurecontainer.io/personal/passive/vip_saving_account/docs/ui</t>
   </si>
 </sst>
 </file>
@@ -847,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EC3994-2505-4875-A4DA-47990DB02DB0}">
   <dimension ref="B1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17:N17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1617,34 +1653,47 @@
         <v>15</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R18" s="6"/>
-      <c r="S18" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1660,34 +1709,47 @@
         <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R19" s="6"/>
-      <c r="S19" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="S19" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -1703,34 +1765,47 @@
         <v>15</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R20" s="6"/>
-      <c r="S20" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="S20" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R21" s="6"/>
@@ -1962,9 +2037,15 @@
     <hyperlink ref="S16" r:id="rId20" xr:uid="{B7AE1AC1-400D-4B10-A802-17331F643E4C}"/>
     <hyperlink ref="R17" r:id="rId21" xr:uid="{93BFB83C-4DA0-44B5-A474-BDAB333C1001}"/>
     <hyperlink ref="S17" r:id="rId22" xr:uid="{99955C05-86B8-435D-8B69-8FD1A572B0A2}"/>
+    <hyperlink ref="R18" r:id="rId23" xr:uid="{4F7E3D5D-E59D-4773-9DAA-1EB0101D5C89}"/>
+    <hyperlink ref="S18" r:id="rId24" xr:uid="{36BE4625-7AFF-4A01-B63A-1379C63BC47F}"/>
+    <hyperlink ref="R19" r:id="rId25" xr:uid="{6445584C-E230-489E-B873-F7DCF394A41B}"/>
+    <hyperlink ref="S19" r:id="rId26" xr:uid="{8B070AB9-4E6A-4AF2-8F55-DDC4E324EB3B}"/>
+    <hyperlink ref="R20" r:id="rId27" xr:uid="{CEE92D5B-0424-42C8-817A-8E28A1625405}"/>
+    <hyperlink ref="S20" r:id="rId28" xr:uid="{B1F19B10-CB31-4397-8702-EE6D6D3B0EDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId29"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>

<commit_message>
proceso de despliegue completado 100%
</commit_message>
<xml_diff>
--- a/desarrollo-microservicios.xlsx
+++ b/desarrollo-microservicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluismen\Documents\BOOTCAMP-BANK-PROJECT\architecture-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE75EF3-F0B4-4645-8B2C-EB89D419D39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AC7BB-096E-41E5-84C5-A451B0FDD223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
   </bookViews>
@@ -884,7 +884,7 @@
   <dimension ref="B1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1674,7 @@
         <v>23</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>23</v>
@@ -1730,7 +1730,7 @@
         <v>23</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>23</v>
@@ -1786,7 +1786,7 @@
         <v>23</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
sonarqube analysis to ms-client
</commit_message>
<xml_diff>
--- a/desarrollo-microservicios.xlsx
+++ b/desarrollo-microservicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluismen\Documents\BOOTCAMP-BANK-PROJECT\architecture-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AC7BB-096E-41E5-84C5-A451B0FDD223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B3CA8D-87EF-4EC2-82FD-5B0FD71CADB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CE994BA-859F-43FE-9DFB-C31C15F42635}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="97">
   <si>
     <t>ms-enterprise-active-credit-card</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>http://gateway-service.eastus.azurecontainer.io/personal/passive/vip_saving_account/docs/ui</t>
+  </si>
+  <si>
+    <t>Lulio</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -884,7 +917,7 @@
   <dimension ref="B1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1204,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>23</v>
@@ -1223,7 +1256,7 @@
       </c>
       <c r="Y8" s="1">
         <f>COUNTIFS(col_estado,ln_completed,col_asignado,X8)/COUNTIFS(col_asignado,X8)</f>
-        <v>0.33333333333333331</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
@@ -1235,18 +1268,15 @@
       <c r="X9" t="s">
         <v>11</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="Y9" s="1" t="e">
         <f>COUNTIFS(col_estado,ln_completed,col_asignado,X9)/COUNTIFS(col_asignado,X9)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
@@ -1303,9 +1333,6 @@
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
       <c r="D11" t="s">
         <v>1</v>
       </c>
@@ -1415,9 +1442,6 @@
       <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
@@ -1475,9 +1499,6 @@
       <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -1531,9 +1552,6 @@
       <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1606,7 @@
         <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -1644,7 +1662,7 @@
         <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -1700,7 +1718,7 @@
         <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -1755,9 +1773,6 @@
       <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
@@ -1948,60 +1963,60 @@
       <c r="S55" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E7 E5 F5:S7 V7:V10 E27:S1048576 E3:S3 R5:R26 E8:S22">
-    <cfRule type="cellIs" dxfId="13" priority="25" operator="equal">
+  <conditionalFormatting sqref="E7 E5 V7:V10 E27:S1048576 E3:S3 R5:R26 E9:S22 F5:S8">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="29" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="30" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:S1048576">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"COMPLETADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"EN PROGRESO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Y5 Y8:Y9">
-    <cfRule type="dataBar" priority="47">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2012,6 +2027,17 @@
           <x14:id>{957D9CE5-77FE-4E92-BE1D-CD7110DE36A5}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"COMPLETADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"EN PROGRESO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"PENDIENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>